<commit_message>
Tudo pronto antes dos tratamentos de erro
</commit_message>
<xml_diff>
--- a/services/infocar/input/teste1.xlsx
+++ b/services/infocar/input/teste1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ma_digitalization\services\infocar\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ma_importer\services\rg_automovel\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE459B6-5733-4ACC-94C5-8C32175BB8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBC08B0-C887-4AE6-881F-2BCF43D55CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Placa</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Consultar Tabela Fipe?</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>S</t>
@@ -90,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -111,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -409,9 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -431,109 +433,112 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+      <c r="A4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+      <c r="A5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>